<commit_message>
Change security tags storage method
Change-Id: I5a8372243424b15916efef39d7b3df670144d3b6
</commit_message>
<xml_diff>
--- a/Doc/TushareApi.xlsx
+++ b/Doc/TushareApi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Private\Code\git\StockAnalysisSystem\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0518C987-F778-414A-9C54-08054BD46730}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB64B19-83C2-4A45-A3D7-557ADC3ED58A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>SaS Uri</t>
   </si>
@@ -58,15 +58,48 @@
   </si>
   <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>无法指定时间参数。
-注意同一家主体在同一天可能存在多笔质押。</t>
   </si>
   <si>
     <t>数据仅在每周五的日期有效。
 无法指定时间范围，同时指定时间及ts_code仅返回当天数据。
 如果仅指定时间，则只返回3000条，没办法将某日所有股票数据获取完整。</t>
+  </si>
+  <si>
+    <t>daily_basic</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=32</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>fina_mainbz</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=81</t>
+  </si>
+  <si>
+    <t>无法指定时间参数。
+注意同一家主体在同一天可能存在多笔质押（将数额也设为主键）。</t>
+  </si>
+  <si>
+    <t>切片更新需要fina_mainbz_vip接口。
+如果不指定type参数，则地区和产品分类会混在一起并且没有字段区分。
+如果不指定时间参数，则返回最近的100条。
+如果指定时间参数，数量过多则返回不超过end_date的最新100条。
+由于每次只能取100条，而每个季度的数量不定，所以应采用时间倒推获取数据。</t>
+  </si>
+  <si>
+    <t>concept_detail</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=126</t>
+  </si>
+  <si>
+    <t>无时间参数。
+可按概念查，也可查股票的概念。
+需要指定字段，默认查询字段不全。</t>
   </si>
 </sst>
 </file>
@@ -398,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G8"/>
+  <dimension ref="B2:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +443,7 @@
     <col min="4" max="4" width="41.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.28515625" customWidth="1"/>
     <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75" customWidth="1"/>
+    <col min="7" max="7" width="82.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
@@ -433,41 +466,86 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="75" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F9" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+      <c r="G9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F10" t="s">
         <v>10</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>11</v>
+      <c r="G10" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1" xr:uid="{7CE395ED-EE8A-432C-97B6-3EE45E56A63E}"/>
-    <hyperlink ref="D8" r:id="rId2" xr:uid="{EDB776CB-98FE-41ED-AA7F-A5419AE90575}"/>
+    <hyperlink ref="D9" r:id="rId1" xr:uid="{7CE395ED-EE8A-432C-97B6-3EE45E56A63E}"/>
+    <hyperlink ref="D10" r:id="rId2" xr:uid="{EDB776CB-98FE-41ED-AA7F-A5419AE90575}"/>
+    <hyperlink ref="D4" r:id="rId3" xr:uid="{D6F62DF8-63C4-4A7E-B244-F5BE829FCFC9}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{5908865A-CA5B-4B24-A1CD-9A333B5D8993}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{CC7049CE-E58C-4003-9963-C55E17BF203E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Arial"&amp;6&amp;K626469Internal</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Adjust the repurchase and unlock collector
Change-Id: I943bf5b9a91d416dc645d73b809e944fa2b560e8
</commit_message>
<xml_diff>
--- a/Doc/TushareApi.xlsx
+++ b/Doc/TushareApi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Private\Code\git\StockAnalysisSystem\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB64B19-83C2-4A45-A3D7-557ADC3ED58A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9B7B16-7EBE-4F8F-8532-75FB98BD3E42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t>SaS Uri</t>
   </si>
@@ -100,6 +100,158 @@
     <t>无时间参数。
 可按概念查，也可查股票的概念。
 需要指定字段，默认查询字段不全。</t>
+  </si>
+  <si>
+    <t>Process</t>
+  </si>
+  <si>
+    <t>Metrics.Stock.Daily</t>
+  </si>
+  <si>
+    <t>Market.SecuritiesTags</t>
+  </si>
+  <si>
+    <t>Finance.BusinessComposition</t>
+  </si>
+  <si>
+    <t>Collector</t>
+  </si>
+  <si>
+    <t>daily_metrics_tushare_pro.py</t>
+  </si>
+  <si>
+    <t>finance_business_tushare_pro.py</t>
+  </si>
+  <si>
+    <t>fina_audit</t>
+  </si>
+  <si>
+    <t>balancesheet</t>
+  </si>
+  <si>
+    <t>income</t>
+  </si>
+  <si>
+    <t>cashflow</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=80</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=36</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=33</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=44</t>
+  </si>
+  <si>
+    <t>finance_data_tushare_pro.py</t>
+  </si>
+  <si>
+    <t>Finance.Audit</t>
+  </si>
+  <si>
+    <t>Finance.BalanceSheet</t>
+  </si>
+  <si>
+    <t>Finance.IncomeStatement</t>
+  </si>
+  <si>
+    <t>Finance.CashFlowStatement</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=95</t>
+  </si>
+  <si>
+    <t>index_daily</t>
+  </si>
+  <si>
+    <t>TradeData.Index.Daily</t>
+  </si>
+  <si>
+    <t>index_data_tushare_pro.py</t>
+  </si>
+  <si>
+    <t>Market.SecuritiesInfo</t>
+  </si>
+  <si>
+    <t>market_data_tushare_pro.py</t>
+  </si>
+  <si>
+    <t>Market.IndexInfo</t>
+  </si>
+  <si>
+    <t>Market.TradeCalender</t>
+  </si>
+  <si>
+    <t>Market.NamingHistory</t>
+  </si>
+  <si>
+    <t>Market.IndexComponent</t>
+  </si>
+  <si>
+    <t>stock_basic</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=25</t>
+  </si>
+  <si>
+    <t>index_basic</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=94</t>
+  </si>
+  <si>
+    <t>TS支持多种指数。
+只选择支持：'SSE', 'SZSE', 'CSI', 'CICC', 'SW', 'MSCI', 'OTH'</t>
+  </si>
+  <si>
+    <t>trade_cal</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=26</t>
+  </si>
+  <si>
+    <t>namechange</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=100</t>
+  </si>
+  <si>
+    <t>指定时间范围可以一次性取完</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>Stockholder.Repurchase</t>
+  </si>
+  <si>
+    <t>Stockholder.StockUnlock</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=124</t>
+  </si>
+  <si>
+    <t>repurchase</t>
+  </si>
+  <si>
+    <t>share_float</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=160</t>
+  </si>
+  <si>
+    <t>repurchase_unlimit_tushare_pro.py</t>
+  </si>
+  <si>
+    <t>一般来说一家公司回购记录很难达到2000条，所以可以认为可以一次性获取所有数据。</t>
+  </si>
+  <si>
+    <t>start_date及end_date参数表现混乱并且不在文档中，不建议使用。
+可以认为一次性获取所有数据。</t>
   </si>
 </sst>
 </file>
@@ -431,121 +583,372 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:G10"/>
+  <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="41.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="82.28515625" customWidth="1"/>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="82.28515625" customWidth="1"/>
+    <col min="9" max="9" width="53.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
       <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="2:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="2:9" ht="75" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
       <c r="C6" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+      <c r="D21" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G21" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
+    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>54</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G22" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>57</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" t="s">
+        <v>10</v>
+      </c>
+      <c r="H25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="G27" t="s">
         <v>14</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>17</v>
+      <c r="H27" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>64</v>
+      </c>
+      <c r="C28" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" t="s">
+        <v>67</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G28" t="s">
+        <v>14</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1" xr:uid="{7CE395ED-EE8A-432C-97B6-3EE45E56A63E}"/>
-    <hyperlink ref="D10" r:id="rId2" xr:uid="{EDB776CB-98FE-41ED-AA7F-A5419AE90575}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{D6F62DF8-63C4-4A7E-B244-F5BE829FCFC9}"/>
-    <hyperlink ref="D7" r:id="rId4" xr:uid="{5908865A-CA5B-4B24-A1CD-9A333B5D8993}"/>
-    <hyperlink ref="D6" r:id="rId5" xr:uid="{CC7049CE-E58C-4003-9963-C55E17BF203E}"/>
+    <hyperlink ref="E8" r:id="rId1" xr:uid="{7CE395ED-EE8A-432C-97B6-3EE45E56A63E}"/>
+    <hyperlink ref="E9" r:id="rId2" xr:uid="{EDB776CB-98FE-41ED-AA7F-A5419AE90575}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{D6F62DF8-63C4-4A7E-B244-F5BE829FCFC9}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{5908865A-CA5B-4B24-A1CD-9A333B5D8993}"/>
+    <hyperlink ref="E21" r:id="rId5" xr:uid="{CC7049CE-E58C-4003-9963-C55E17BF203E}"/>
+    <hyperlink ref="E12" r:id="rId6" xr:uid="{26CA76AA-00CD-405A-AE4F-11B55639E22C}"/>
+    <hyperlink ref="E13" r:id="rId7" xr:uid="{262DBF26-2943-4B39-BDC5-DB9E1D73760E}"/>
+    <hyperlink ref="E14" r:id="rId8" xr:uid="{196F4EE0-08F2-4C98-8378-03253FB2A203}"/>
+    <hyperlink ref="E15" r:id="rId9" xr:uid="{43B4EE18-1AE2-4037-9182-1E60D33D99F6}"/>
+    <hyperlink ref="E17" r:id="rId10" xr:uid="{AC4FFEE6-3673-422D-9144-C76945E08886}"/>
+    <hyperlink ref="E20" r:id="rId11" xr:uid="{53497F0E-CC79-4CEC-9C7A-8C1BE5154BF5}"/>
+    <hyperlink ref="E22" r:id="rId12" xr:uid="{F4E62DFD-4C30-4C30-99F5-BDACB1197F0F}"/>
+    <hyperlink ref="E23" r:id="rId13" xr:uid="{B806FBD2-A615-468D-89EF-C2559F19F068}"/>
+    <hyperlink ref="E24" r:id="rId14" xr:uid="{1D136DBF-033F-494D-BF8B-AB68E2DA4DF0}"/>
+    <hyperlink ref="E27" r:id="rId15" xr:uid="{11FDC3CC-6430-4F3F-9446-4FBFA1630367}"/>
+    <hyperlink ref="E28" r:id="rId16" xr:uid="{BE98706B-5794-431F-A5F2-1D49459E7AA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Arial"&amp;6&amp;K626469Internal</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Improve the stock holder data process.
Change-Id: I49b58f0c825773cba0226473c493270a910649e9
</commit_message>
<xml_diff>
--- a/Doc/TushareApi.xlsx
+++ b/Doc/TushareApi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Private\Code\git\StockAnalysisSystem\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\d\private\code\git\stockanalysissystem\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE9B7B16-7EBE-4F8F-8532-75FB98BD3E42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585C6852-4823-4798-93E7-FD227568AEDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
   <si>
     <t>SaS Uri</t>
   </si>
@@ -58,11 +58,6 @@
   </si>
   <si>
     <t>NO</t>
-  </si>
-  <si>
-    <t>数据仅在每周五的日期有效。
-无法指定时间范围，同时指定时间及ts_code仅返回当天数据。
-如果仅指定时间，则只返回3000条，没办法将某日所有股票数据获取完整。</t>
   </si>
   <si>
     <t>daily_basic</t>
@@ -252,6 +247,66 @@
   <si>
     <t>start_date及end_date参数表现混乱并且不在文档中，不建议使用。
 可以认为一次性获取所有数据。</t>
+  </si>
+  <si>
+    <t>stockholder_data_tushare_pro.py</t>
+  </si>
+  <si>
+    <t>Stockholder.PledgeStatus</t>
+  </si>
+  <si>
+    <t>Stockholder.PledgeHistory</t>
+  </si>
+  <si>
+    <t>数据仅在每周五的日期有效。
+无法指定时间范围，无法仅指定时间。
+同时指定时间及ts_code仅返回当天数据。
+如果仅指定时间，则只返回3000条，没办法将某日所有股票数据获取完整。</t>
+  </si>
+  <si>
+    <t>stk_holdernumber</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=166</t>
+  </si>
+  <si>
+    <t>top10_holders</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=61</t>
+  </si>
+  <si>
+    <t>top10_floatholders</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=62</t>
+  </si>
+  <si>
+    <t>Stockholder.Statistics</t>
+  </si>
+  <si>
+    <t>5000积分，仅指定ann_date或end_date能够返回4500条。
+5000积分单股票可以一次性取到91条，从1993年1月开始（600651）。
+然而ann_date和end_date都非报告周期（非固定时间）。</t>
+  </si>
+  <si>
+    <t>5000积分单股票可以一次性取到1000多条，从1993年1月开始（600651）。
+可以仅指定日期，但是仅返回5000条，无法取得当期所有股票数据。
+ann_date不确定，报告周期体现在end_date中。</t>
+  </si>
+  <si>
+    <t>5000积分单股票可以一次性取到700多条，从2004年4月开始（600651）。
+可以仅指定日期，但是仅返回5000条，无法取得当期所有股票数据。
+ann_date不确定，报告周期体现在end_date中。</t>
+  </si>
+  <si>
+    <t>https://tushare.pro/document/2?doc_id=175</t>
+  </si>
+  <si>
+    <t>stk_holdertrade</t>
+  </si>
+  <si>
+    <t>Stockholder.ReductionIncrease</t>
   </si>
 </sst>
 </file>
@@ -583,15 +638,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:I28"/>
+  <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="41.7109375" bestFit="1" customWidth="1"/>
@@ -606,7 +661,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>1</v>
@@ -624,24 +679,24 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="G4" t="s">
         <v>13</v>
-      </c>
-      <c r="G4" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
@@ -649,306 +704,398 @@
     </row>
     <row r="6" spans="2:9" ht="75" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="D6" t="s">
-        <v>15</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" t="s">
-        <v>14</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="2:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="G8" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="G9" t="s">
-        <v>10</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" t="s">
-        <v>10</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="G13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G15" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>51</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>42</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G19" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" t="s">
         <v>46</v>
       </c>
-      <c r="C20" t="s">
-        <v>47</v>
-      </c>
       <c r="D20" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G20" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="21" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="H20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" t="s">
-        <v>19</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="G21" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="2:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>56</v>
+      <c r="H21" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C23" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
       <c r="G23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="H23" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>68</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="G24" t="s">
-        <v>10</v>
-      </c>
-      <c r="H24" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" t="s">
-        <v>47</v>
-      </c>
-      <c r="G25" t="s">
-        <v>10</v>
-      </c>
-      <c r="H25" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C27" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D27" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>65</v>
+        <v>9</v>
       </c>
       <c r="G27" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="28" spans="2:8" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C28" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="G28" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H28" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>81</v>
+      </c>
+      <c r="C29" t="s">
         <v>71</v>
+      </c>
+      <c r="D29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G29" t="s">
+        <v>10</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>81</v>
+      </c>
+      <c r="C30" t="s">
+        <v>71</v>
+      </c>
+      <c r="D30" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G30" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>87</v>
+      </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" t="s">
+        <v>86</v>
+      </c>
+      <c r="E31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E8" r:id="rId1" xr:uid="{7CE395ED-EE8A-432C-97B6-3EE45E56A63E}"/>
-    <hyperlink ref="E9" r:id="rId2" xr:uid="{EDB776CB-98FE-41ED-AA7F-A5419AE90575}"/>
+    <hyperlink ref="E26" r:id="rId1" xr:uid="{7CE395ED-EE8A-432C-97B6-3EE45E56A63E}"/>
+    <hyperlink ref="E27" r:id="rId2" xr:uid="{EDB776CB-98FE-41ED-AA7F-A5419AE90575}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{D6F62DF8-63C4-4A7E-B244-F5BE829FCFC9}"/>
     <hyperlink ref="E6" r:id="rId4" xr:uid="{5908865A-CA5B-4B24-A1CD-9A333B5D8993}"/>
-    <hyperlink ref="E21" r:id="rId5" xr:uid="{CC7049CE-E58C-4003-9963-C55E17BF203E}"/>
-    <hyperlink ref="E12" r:id="rId6" xr:uid="{26CA76AA-00CD-405A-AE4F-11B55639E22C}"/>
-    <hyperlink ref="E13" r:id="rId7" xr:uid="{262DBF26-2943-4B39-BDC5-DB9E1D73760E}"/>
-    <hyperlink ref="E14" r:id="rId8" xr:uid="{196F4EE0-08F2-4C98-8378-03253FB2A203}"/>
-    <hyperlink ref="E15" r:id="rId9" xr:uid="{43B4EE18-1AE2-4037-9182-1E60D33D99F6}"/>
-    <hyperlink ref="E17" r:id="rId10" xr:uid="{AC4FFEE6-3673-422D-9144-C76945E08886}"/>
-    <hyperlink ref="E20" r:id="rId11" xr:uid="{53497F0E-CC79-4CEC-9C7A-8C1BE5154BF5}"/>
-    <hyperlink ref="E22" r:id="rId12" xr:uid="{F4E62DFD-4C30-4C30-99F5-BDACB1197F0F}"/>
-    <hyperlink ref="E23" r:id="rId13" xr:uid="{B806FBD2-A615-468D-89EF-C2559F19F068}"/>
-    <hyperlink ref="E24" r:id="rId14" xr:uid="{1D136DBF-033F-494D-BF8B-AB68E2DA4DF0}"/>
-    <hyperlink ref="E27" r:id="rId15" xr:uid="{11FDC3CC-6430-4F3F-9446-4FBFA1630367}"/>
-    <hyperlink ref="E28" r:id="rId16" xr:uid="{BE98706B-5794-431F-A5F2-1D49459E7AA8}"/>
+    <hyperlink ref="E17" r:id="rId5" xr:uid="{CC7049CE-E58C-4003-9963-C55E17BF203E}"/>
+    <hyperlink ref="E8" r:id="rId6" xr:uid="{26CA76AA-00CD-405A-AE4F-11B55639E22C}"/>
+    <hyperlink ref="E9" r:id="rId7" xr:uid="{262DBF26-2943-4B39-BDC5-DB9E1D73760E}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{196F4EE0-08F2-4C98-8378-03253FB2A203}"/>
+    <hyperlink ref="E11" r:id="rId9" xr:uid="{43B4EE18-1AE2-4037-9182-1E60D33D99F6}"/>
+    <hyperlink ref="E13" r:id="rId10" xr:uid="{AC4FFEE6-3673-422D-9144-C76945E08886}"/>
+    <hyperlink ref="E16" r:id="rId11" xr:uid="{53497F0E-CC79-4CEC-9C7A-8C1BE5154BF5}"/>
+    <hyperlink ref="E18" r:id="rId12" xr:uid="{F4E62DFD-4C30-4C30-99F5-BDACB1197F0F}"/>
+    <hyperlink ref="E19" r:id="rId13" xr:uid="{B806FBD2-A615-468D-89EF-C2559F19F068}"/>
+    <hyperlink ref="E20" r:id="rId14" xr:uid="{1D136DBF-033F-494D-BF8B-AB68E2DA4DF0}"/>
+    <hyperlink ref="E23" r:id="rId15" xr:uid="{11FDC3CC-6430-4F3F-9446-4FBFA1630367}"/>
+    <hyperlink ref="E24" r:id="rId16" xr:uid="{BE98706B-5794-431F-A5F2-1D49459E7AA8}"/>
+    <hyperlink ref="E28" r:id="rId17" xr:uid="{08988B55-7260-4BE6-AA28-8378B4C1E4C5}"/>
+    <hyperlink ref="E29" r:id="rId18" xr:uid="{C4F5321C-9213-4466-A851-3965EE4CA4DC}"/>
+    <hyperlink ref="E30" r:id="rId19" xr:uid="{B5E6FF03-DF0A-4378-8E91-834D8DA16D84}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId17"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Arial"&amp;6&amp;K626469Internal</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Improve ReductionIncrease data collector
Change-Id: Icfac7686ee1361f63d04d97cf54cc17194f1e2c3
</commit_message>
<xml_diff>
--- a/Doc/TushareApi.xlsx
+++ b/Doc/TushareApi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="c:\d\private\code\git\stockanalysissystem\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Private\Code\git\StockAnalysisSystem\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{585C6852-4823-4798-93E7-FD227568AEDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165D21D8-8964-4E4A-A29F-B593F86A4025}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="89">
   <si>
     <t>SaS Uri</t>
   </si>
@@ -307,6 +307,11 @@
   </si>
   <si>
     <t>Stockholder.ReductionIncrease</t>
+  </si>
+  <si>
+    <t>可以按日获取当日所有增减持数据。
+一个股票某日可以有多个主体增减持，所以需要将holder_name加入主键
+一般一个股票很难达到3000条数据，可以视为能一次性取完单股历史数据</t>
   </si>
 </sst>
 </file>
@@ -641,7 +646,7 @@
   <dimension ref="B2:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,7 +1060,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" ht="45" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>87</v>
       </c>
@@ -1065,11 +1070,14 @@
       <c r="D31" t="s">
         <v>86</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G31" t="s">
         <v>10</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1093,9 +1101,10 @@
     <hyperlink ref="E28" r:id="rId17" xr:uid="{08988B55-7260-4BE6-AA28-8378B4C1E4C5}"/>
     <hyperlink ref="E29" r:id="rId18" xr:uid="{C4F5321C-9213-4466-A851-3965EE4CA4DC}"/>
     <hyperlink ref="E30" r:id="rId19" xr:uid="{B5E6FF03-DF0A-4378-8E91-834D8DA16D84}"/>
+    <hyperlink ref="E31" r:id="rId20" xr:uid="{99F75474-0718-4EA1-88E0-C61A2A8DA6EB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId20"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId21"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;1#&amp;"Arial"&amp;6&amp;K626469Internal</oddFooter>
   </headerFooter>

</xml_diff>